<commit_message>
New CI Pipeline created on GitLab
</commit_message>
<xml_diff>
--- a/documents/tourguidePerformanceGraph.xlsx
+++ b/documents/tourguidePerformanceGraph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylance\Desktop\Formation OpenClassrooms\P8 - Améliorez votre application avec des systèmes distribués\Projet 8 - TourGuide Application\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF94BA1-7232-4CFD-96CC-B65BCDB628C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD2C41-74FF-4FB7-8261-8F67F477930B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="2775" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.86099999999999999</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.3050000000000002</c:v>
@@ -306,7 +306,7 @@
                   <c:v>102.08199999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>204.30600000000001</c:v>
+                  <c:v>203.755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,7 +662,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.5449999999999999</c:v>
+                  <c:v>1.677</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.709</c:v>
@@ -671,7 +671,7 @@
                   <c:v>102.33199999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1022.742</c:v>
+                  <c:v>1026.4100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1">
-        <v>0.86099999999999999</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1322,7 +1322,7 @@
         <v>7579</v>
       </c>
       <c r="D8" s="1">
-        <v>204.30600000000001</v>
+        <v>203.755</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1339,7 @@
   <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1366,7 +1366,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="1">
-        <v>1.5449999999999999</v>
+        <v>1.677</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1399,7 +1399,7 @@
         <v>64020</v>
       </c>
       <c r="D6" s="1">
-        <v>1022.742</v>
+        <v>1026.4100000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last code refactored. Javadoc updated. New performance tests done. Graph doc updated.
</commit_message>
<xml_diff>
--- a/documents/tourguidePerformanceGraph.xlsx
+++ b/documents/tourguidePerformanceGraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylance\Desktop\Formation OpenClassrooms\P8 - Améliorez votre application avec des systèmes distribués\Projet 8 - TourGuide Application\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD2C41-74FF-4FB7-8261-8F67F477930B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BFB5CA-A519-4B8A-B0B1-BF0FA30622EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4860" yWindow="2775" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,6 +42,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -84,12 +87,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,25 +292,25 @@
             <c:numRef>
               <c:f>Locations!$D$3:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.89</c:v>
+                  <c:v>0.83499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3050000000000002</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.308</c:v>
+                  <c:v>10.250999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.463000000000001</c:v>
+                  <c:v>20.478999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.08199999999999</c:v>
+                  <c:v>102.065</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>203.755</c:v>
+                  <c:v>204.26300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -659,19 +663,19 @@
             <c:numRef>
               <c:f>Rewards!$D$3:$D$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.677</c:v>
+                  <c:v>1.6379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.709</c:v>
+                  <c:v>11.039</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.33199999999999</c:v>
+                  <c:v>103.76600000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1026.4100000000001</c:v>
+                  <c:v>1022.355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1236,10 +1240,14 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
@@ -1266,8 +1274,8 @@
       <c r="C3" s="1">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.89</v>
+      <c r="D3" s="3">
+        <v>0.83499999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1277,8 +1285,8 @@
       <c r="C4" s="1">
         <v>75</v>
       </c>
-      <c r="D4" s="1">
-        <v>2.3050000000000002</v>
+      <c r="D4" s="3">
+        <v>2.33</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1288,8 +1296,8 @@
       <c r="C5" s="1">
         <v>376</v>
       </c>
-      <c r="D5" s="1">
-        <v>10.308</v>
+      <c r="D5" s="3">
+        <v>10.250999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1299,8 +1307,8 @@
       <c r="C6" s="1">
         <v>762</v>
       </c>
-      <c r="D6" s="1">
-        <v>20.463000000000001</v>
+      <c r="D6" s="3">
+        <v>20.478999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1310,8 +1318,8 @@
       <c r="C7" s="1">
         <v>3791</v>
       </c>
-      <c r="D7" s="1">
-        <v>102.08199999999999</v>
+      <c r="D7" s="3">
+        <v>102.065</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1321,8 +1329,8 @@
       <c r="C8" s="1">
         <v>7579</v>
       </c>
-      <c r="D8" s="1">
-        <v>203.755</v>
+      <c r="D8" s="3">
+        <v>204.26300000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1365,8 +1373,8 @@
       <c r="C3" s="1">
         <v>44</v>
       </c>
-      <c r="D3" s="1">
-        <v>1.677</v>
+      <c r="D3" s="3">
+        <v>1.6379999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1376,8 +1384,8 @@
       <c r="C4" s="1">
         <v>472</v>
       </c>
-      <c r="D4" s="1">
-        <v>10.709</v>
+      <c r="D4" s="3">
+        <v>11.039</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,8 +1395,8 @@
       <c r="C5" s="1">
         <v>5820</v>
       </c>
-      <c r="D5" s="1">
-        <v>102.33199999999999</v>
+      <c r="D5" s="3">
+        <v>103.76600000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1398,8 +1406,8 @@
       <c r="C6" s="1">
         <v>64020</v>
       </c>
-      <c r="D6" s="1">
-        <v>1026.4100000000001</v>
+      <c r="D6" s="3">
+        <v>1022.355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>